<commit_message>
added ingredients to the base_resources
</commit_message>
<xml_diff>
--- a/base_resources.xlsx
+++ b/base_resources.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="75">
   <si>
     <t>name</t>
   </si>
@@ -133,6 +133,114 @@
   </si>
   <si>
     <t>pumpjack</t>
+  </si>
+  <si>
+    <t>depleted-uranium-fuel-cell</t>
+  </si>
+  <si>
+    <t>ammoniacal-solution</t>
+  </si>
+  <si>
+    <t>wood</t>
+  </si>
+  <si>
+    <t>biter-egg</t>
+  </si>
+  <si>
+    <t>tungsten-ore</t>
+  </si>
+  <si>
+    <t>promethium-asteroid-chunk</t>
+  </si>
+  <si>
+    <t>lava</t>
+  </si>
+  <si>
+    <t>yumako</t>
+  </si>
+  <si>
+    <t>jellynut</t>
+  </si>
+  <si>
+    <t>scrap</t>
+  </si>
+  <si>
+    <t>nuclear-fuel-reprocessing</t>
+  </si>
+  <si>
+    <t>nuclear-reactor</t>
+  </si>
+  <si>
+    <t>power-generation</t>
+  </si>
+  <si>
+    <t>uranium-fuel-cell</t>
+  </si>
+  <si>
+    <t>offshore-pumping</t>
+  </si>
+  <si>
+    <t>offshore-pump</t>
+  </si>
+  <si>
+    <t>harvesting</t>
+  </si>
+  <si>
+    <t>player</t>
+  </si>
+  <si>
+    <t>big-mining-drill</t>
+  </si>
+  <si>
+    <t>asteroid-mining</t>
+  </si>
+  <si>
+    <t>asteroid-collector</t>
+  </si>
+  <si>
+    <t>metallic-asteroid-chunk</t>
+  </si>
+  <si>
+    <t>carbonic-asteroid-chunk</t>
+  </si>
+  <si>
+    <t>oxide-asteroid-chunk</t>
+  </si>
+  <si>
+    <t>raw-fish</t>
+  </si>
+  <si>
+    <t>pentapod-egg</t>
+  </si>
+  <si>
+    <t>metallic-asteroid-chunk-asteroid</t>
+  </si>
+  <si>
+    <t>carbonic-asteroid-chunk-asteroid</t>
+  </si>
+  <si>
+    <t>oxide-asteroid-chunk-asteroid</t>
+  </si>
+  <si>
+    <t>promethium-asteroid-chunk-asteroid</t>
+  </si>
+  <si>
+    <t>wood-harvesting</t>
+  </si>
+  <si>
+    <t>biter-egg-harvesting</t>
+  </si>
+  <si>
+    <t>yumako-harvesting</t>
+  </si>
+  <si>
+    <t>jellynut-harvesting</t>
+  </si>
+  <si>
+    <t>raw-fish-harvesting</t>
+  </si>
+  <si>
+    <t>pentapod-egg-harvesting</t>
   </si>
 </sst>
 </file>
@@ -464,14 +572,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S11"/>
+  <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
+    <col min="1" max="1" width="20.265625" customWidth="1"/>
     <col min="3" max="3" width="12.59765625" customWidth="1"/>
     <col min="7" max="7" width="13.3984375" customWidth="1"/>
     <col min="8" max="8" width="13.53125" customWidth="1"/>
@@ -597,10 +706,10 @@
         <v>3</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -702,10 +811,10 @@
         <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="E5">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F5" t="s">
         <v>30</v>
@@ -717,13 +826,13 @@
         <v>21</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>1200</v>
       </c>
       <c r="J5" t="s">
         <v>33</v>
       </c>
       <c r="O5" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="P5">
         <v>1</v>
@@ -999,8 +1108,684 @@
         <v>0</v>
       </c>
     </row>
+    <row r="12" spans="1:19">
+      <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12">
+        <v>1011</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12">
+        <v>200</v>
+      </c>
+      <c r="F12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>39</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>34</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12" t="s">
+        <v>52</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12" t="s">
+        <v>34</v>
+      </c>
+      <c r="O12" t="s">
+        <v>50</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>6</v>
+      </c>
+      <c r="R12">
+        <v>7</v>
+      </c>
+      <c r="S12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13">
+        <v>1012</v>
+      </c>
+      <c r="C13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13" t="s">
+        <v>40</v>
+      </c>
+      <c r="I13">
+        <v>1200</v>
+      </c>
+      <c r="J13" t="s">
+        <v>33</v>
+      </c>
+      <c r="O13" t="s">
+        <v>54</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="A14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14">
+        <v>1013</v>
+      </c>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
+        <v>41</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14" t="s">
+        <v>34</v>
+      </c>
+      <c r="O14" t="s">
+        <v>56</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15">
+        <v>1014</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15" t="s">
+        <v>42</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15" t="s">
+        <v>34</v>
+      </c>
+      <c r="O15" t="s">
+        <v>56</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16">
+        <v>1015</v>
+      </c>
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16">
+        <v>5</v>
+      </c>
+      <c r="F16" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>43</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16" t="s">
+        <v>34</v>
+      </c>
+      <c r="O16" t="s">
+        <v>57</v>
+      </c>
+      <c r="P16">
+        <v>2.5</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19">
+      <c r="A17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17">
+        <v>1016</v>
+      </c>
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17" t="s">
+        <v>44</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17" t="s">
+        <v>34</v>
+      </c>
+      <c r="O17" t="s">
+        <v>59</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19">
+      <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18">
+        <v>1017</v>
+      </c>
+      <c r="C18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
+        <v>45</v>
+      </c>
+      <c r="I18">
+        <v>1200</v>
+      </c>
+      <c r="J18" t="s">
+        <v>33</v>
+      </c>
+      <c r="O18" t="s">
+        <v>54</v>
+      </c>
+      <c r="P18">
+        <v>1</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19">
+      <c r="A19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19">
+        <v>1018</v>
+      </c>
+      <c r="C19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19" t="s">
+        <v>46</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19" t="s">
+        <v>34</v>
+      </c>
+      <c r="O19" t="s">
+        <v>56</v>
+      </c>
+      <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19">
+      <c r="A20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20">
+        <v>1019</v>
+      </c>
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20" t="s">
+        <v>47</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20" t="s">
+        <v>34</v>
+      </c>
+      <c r="O20" t="s">
+        <v>56</v>
+      </c>
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19">
+      <c r="A21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21">
+        <v>1020</v>
+      </c>
+      <c r="C21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21" t="s">
+        <v>48</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21" t="s">
+        <v>34</v>
+      </c>
+      <c r="O21" t="s">
+        <v>37</v>
+      </c>
+      <c r="P21">
+        <v>0.5</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19">
+      <c r="A22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22">
+        <v>1021</v>
+      </c>
+      <c r="C22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22" t="s">
+        <v>60</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22" t="s">
+        <v>34</v>
+      </c>
+      <c r="O22" t="s">
+        <v>59</v>
+      </c>
+      <c r="P22">
+        <v>1</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19">
+      <c r="A23" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23">
+        <v>1022</v>
+      </c>
+      <c r="C23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" t="s">
+        <v>58</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23" t="s">
+        <v>30</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23" t="s">
+        <v>61</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23" t="s">
+        <v>34</v>
+      </c>
+      <c r="O23" t="s">
+        <v>59</v>
+      </c>
+      <c r="P23">
+        <v>1</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19">
+      <c r="A24" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24">
+        <v>1023</v>
+      </c>
+      <c r="C24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
+        <v>30</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24" t="s">
+        <v>62</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24" t="s">
+        <v>34</v>
+      </c>
+      <c r="O24" t="s">
+        <v>59</v>
+      </c>
+      <c r="P24">
+        <v>1</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="S24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19">
+      <c r="A25" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25">
+        <v>1024</v>
+      </c>
+      <c r="C25" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
+        <v>30</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25" t="s">
+        <v>63</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25" t="s">
+        <v>34</v>
+      </c>
+      <c r="O25" t="s">
+        <v>56</v>
+      </c>
+      <c r="P25">
+        <v>1</v>
+      </c>
+      <c r="R25">
+        <v>0</v>
+      </c>
+      <c r="S25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19">
+      <c r="A26" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26">
+        <v>1025</v>
+      </c>
+      <c r="C26" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" t="s">
+        <v>55</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>30</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26" t="s">
+        <v>64</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26" t="s">
+        <v>34</v>
+      </c>
+      <c r="O26" t="s">
+        <v>56</v>
+      </c>
+      <c r="P26">
+        <v>1</v>
+      </c>
+      <c r="R26">
+        <v>0</v>
+      </c>
+      <c r="S26">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>